<commit_message>
feedback verwerkt (deels) + deploytimes
</commit_message>
<xml_diff>
--- a/R/deploytimes/results_test.xlsx
+++ b/R/deploytimes/results_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28700" windowHeight="16040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="65">
   <si>
     <t>Anode7</t>
   </si>
@@ -219,13 +219,16 @@
   </si>
   <si>
     <t>40--41</t>
+  </si>
+  <si>
+    <t>21-22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -238,13 +241,24 @@
       <color rgb="FF161B1F"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -259,16 +273,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -297,6 +319,37 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -320,30 +373,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$B$54:$H$54</c:f>
+              <c:f>Blad1!$C$9:$F$9</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7.41</c:v>
+                  <c:v>16.93</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.7</c:v>
+                  <c:v>9.55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.2</c:v>
+                  <c:v>16.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.44</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20.33</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.29</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.41</c:v>
+                  <c:v>9.96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -367,33 +411,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$B$68:$I$68</c:f>
+              <c:f>Blad1!$D$24:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8.54</c:v>
+                  <c:v>14.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.75</c:v>
+                  <c:v>13.97</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.99</c:v>
+                  <c:v>13.31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.98</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.17</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22.9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.66</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.85</c:v>
+                  <c:v>18.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -417,33 +449,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$B$82:$I$82</c:f>
+              <c:f>Blad1!$D$39:$G$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7.94</c:v>
+                  <c:v>29.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.53</c:v>
+                  <c:v>37.83</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.73</c:v>
+                  <c:v>56.36</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.91</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.13</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22.99</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.63</c:v>
+                  <c:v>48.62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -467,39 +487,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$B$96:$K$96</c:f>
+              <c:f>Blad1!$D$54:$G$54</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>17.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.78</c:v>
+                  <c:v>10.44</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.36</c:v>
+                  <c:v>20.33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10.84</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11.14</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20.48</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10.18</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6.713</c:v>
+                  <c:v>11.29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -523,36 +525,154 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$B$110:$J$110</c:f>
+              <c:f>Blad1!$D$68:$H$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$82:$G$82</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6.86</c:v>
+                  <c:v>11.73</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.69</c:v>
+                  <c:v>18.91</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>11.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$96:$J$96</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>9.36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.84</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$110:$H$110</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
                   <c:v>12.1</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.82</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.54</c:v>
+                  <c:v>8.45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.82</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.45</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>23.25</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.99</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -568,17 +688,16 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1210265584"/>
-        <c:axId val="1213480688"/>
+        <c:axId val="1242274512"/>
+        <c:axId val="1242276560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1210265584"/>
+        <c:axId val="1242274512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -615,7 +734,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1213480688"/>
+        <c:crossAx val="1242276560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -623,7 +742,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1213480688"/>
+        <c:axId val="1242276560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -643,6 +762,37 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -673,10 +823,655 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1210265584"/>
+        <c:crossAx val="1242274512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$C$13:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>41.64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$26:$G$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>41.64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.43</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$41:$G$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>36.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53.24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52.62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$56:$G$56</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>43.73</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56.69</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52.82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$70:$H$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>37.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53.08</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31.59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$84:$G$84</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>39.42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55.15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$98:$J$98</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>45.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56.86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47.35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.53</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$112:$H$112</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.79</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31.59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1213650832"/>
+        <c:axId val="1241694112"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1213650832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1241694112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1241694112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1213650832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -762,6 +1557,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1278,24 +2113,540 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Grafiek 1"/>
+        <xdr:cNvPr id="3" name="Grafiek 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1305,6 +2656,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Grafiek 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1578,8 +2959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:K114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="F20" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1630,7 +3011,7 @@
       <c r="F8" t="s">
         <v>8</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1638,7 +3019,7 @@
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="8">
         <v>11.53</v>
       </c>
       <c r="C9" s="3">
@@ -1653,15 +3034,23 @@
       <c r="F9" s="3">
         <v>9.9600000000000009</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="8">
         <v>8.9600000000000009</v>
       </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="9"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="9"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="9">
         <v>0.39</v>
       </c>
       <c r="C12">
@@ -1676,7 +3065,7 @@
       <c r="F12">
         <v>0.52</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="9">
         <v>0.43</v>
       </c>
     </row>
@@ -1684,7 +3073,7 @@
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="9">
         <v>29.04</v>
       </c>
       <c r="C13">
@@ -1699,7 +3088,7 @@
       <c r="F13">
         <v>31.78</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="9">
         <v>31.69</v>
       </c>
     </row>
@@ -1707,7 +3096,7 @@
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="9">
         <v>4169</v>
       </c>
       <c r="C14">
@@ -1722,7 +3111,7 @@
       <c r="F14">
         <v>4259</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="9">
         <v>4120</v>
       </c>
     </row>
@@ -1730,7 +3119,7 @@
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="9">
         <v>307</v>
       </c>
       <c r="C15">
@@ -1745,7 +3134,7 @@
       <c r="F15">
         <v>0</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1785,10 +3174,10 @@
       <c r="B22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
+      <c r="B23" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D23" t="s">
@@ -1800,18 +3189,19 @@
       <c r="F23" t="s">
         <v>21</v>
       </c>
-      <c r="G23" t="s">
-        <v>22</v>
-      </c>
+      <c r="G23" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="9">
         <v>7.46</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="9">
         <v>943</v>
       </c>
       <c r="D24">
@@ -1823,10 +3213,10 @@
       <c r="F24">
         <v>13.31</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="11">
         <v>18.55</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="9">
         <v>9.5500000000000007</v>
       </c>
     </row>
@@ -1834,10 +3224,10 @@
       <c r="A25" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="10">
         <v>0</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="9">
         <v>0.04</v>
       </c>
       <c r="D25">
@@ -1849,10 +3239,10 @@
       <c r="F25">
         <v>0.27</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="11">
         <v>0.31</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="9">
         <v>0.11</v>
       </c>
     </row>
@@ -1860,10 +3250,10 @@
       <c r="A26" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="10">
         <v>29.01</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="9">
         <v>29.06</v>
       </c>
       <c r="D26">
@@ -1875,10 +3265,10 @@
       <c r="F26">
         <v>52.84</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="11">
         <v>31.43</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="9">
         <v>31.4</v>
       </c>
     </row>
@@ -1886,10 +3276,10 @@
       <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="9">
         <v>36606</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="9">
         <v>3577</v>
       </c>
       <c r="D27">
@@ -1901,10 +3291,10 @@
       <c r="F27">
         <v>13481</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="11">
         <v>4495</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="9">
         <v>4191</v>
       </c>
     </row>
@@ -1912,10 +3302,10 @@
       <c r="A28" t="s">
         <v>14</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="9">
         <v>0</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="9">
         <v>88</v>
       </c>
       <c r="D28">
@@ -1927,10 +3317,10 @@
       <c r="F28">
         <v>0</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="11">
         <v>247</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1970,10 +3360,10 @@
       <c r="B37" s="1"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+      <c r="B38" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D38" t="s">
@@ -1988,36 +3378,37 @@
       <c r="G38" t="s">
         <v>29</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="9" t="s">
         <v>4</v>
       </c>
+      <c r="I38" s="9"/>
     </row>
     <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="13">
         <v>29.13</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="14">
         <v>29.03</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="5">
         <v>29.02</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="5">
         <v>37.83</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="5">
         <v>56.36</v>
       </c>
-      <c r="G39" s="6">
+      <c r="G39" s="5">
         <v>48.62</v>
       </c>
-      <c r="H39" s="6">
+      <c r="H39" s="15">
         <v>31.61</v>
       </c>
-      <c r="I39" s="6">
+      <c r="I39" s="15">
         <v>31.63</v>
       </c>
     </row>
@@ -2025,28 +3416,28 @@
       <c r="A40" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="14">
         <v>0</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40" s="14">
         <v>0</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="5">
         <v>0.11</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="5">
         <v>0.09</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40" s="5">
         <v>0.24</v>
       </c>
-      <c r="G40" s="6">
+      <c r="G40" s="5">
         <v>0.17</v>
       </c>
-      <c r="H40" s="6">
+      <c r="H40" s="15">
         <v>0.09</v>
       </c>
-      <c r="I40" s="6">
+      <c r="I40" s="15">
         <v>0.03</v>
       </c>
     </row>
@@ -2054,28 +3445,28 @@
       <c r="A41" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="14">
         <v>29.05</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="14">
         <v>29.02</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="5">
         <v>36.520000000000003</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="5">
         <v>53.24</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41" s="5">
         <v>52.62</v>
       </c>
-      <c r="G41" s="6">
+      <c r="G41" s="5">
         <v>31.61</v>
       </c>
-      <c r="H41" s="6">
+      <c r="H41" s="15">
         <v>31.62</v>
       </c>
-      <c r="I41" s="6">
+      <c r="I41" s="15">
         <v>31.65</v>
       </c>
     </row>
@@ -2083,10 +3474,10 @@
       <c r="A42" t="s">
         <v>13</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="12">
         <v>0</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="12">
         <v>0</v>
       </c>
       <c r="D42">
@@ -2101,10 +3492,10 @@
       <c r="G42">
         <v>240</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="9">
         <v>0</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="9">
         <v>0</v>
       </c>
     </row>
@@ -2112,10 +3503,10 @@
       <c r="A43" t="s">
         <v>14</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="12">
         <v>3639</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="12">
         <v>3636</v>
       </c>
       <c r="D43">
@@ -2130,10 +3521,10 @@
       <c r="G43">
         <v>5511</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="9">
         <v>4201</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="9">
         <v>4142</v>
       </c>
     </row>
@@ -2170,10 +3561,10 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
+      <c r="B53" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="9" t="s">
         <v>32</v>
       </c>
       <c r="D53" t="s">
@@ -2188,7 +3579,7 @@
       <c r="G53" t="s">
         <v>36</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H53" s="9" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2196,25 +3587,25 @@
       <c r="A54" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B54" s="10">
         <v>7.41</v>
       </c>
-      <c r="C54" s="6">
+      <c r="C54" s="15">
         <v>8.6999999999999993</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D54" s="5">
         <v>17.2</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E54" s="5">
         <v>10.44</v>
       </c>
-      <c r="F54" s="6">
+      <c r="F54" s="5">
         <v>20.329999999999998</v>
       </c>
-      <c r="G54" s="6">
+      <c r="G54" s="5">
         <v>11.29</v>
       </c>
-      <c r="H54" s="6">
+      <c r="H54" s="15">
         <v>9.41</v>
       </c>
     </row>
@@ -2222,64 +3613,64 @@
       <c r="A55" t="s">
         <v>11</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="15">
         <v>0.4</v>
       </c>
-      <c r="C55" s="6">
+      <c r="C55" s="15">
         <v>0.36</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D55" s="5">
         <v>0.5</v>
       </c>
-      <c r="E55" s="6">
+      <c r="E55" s="5">
         <v>0.6</v>
       </c>
-      <c r="F55" s="6">
+      <c r="F55" s="5">
         <v>0.67</v>
       </c>
-      <c r="G55" s="6">
+      <c r="G55" s="5">
         <v>0.59</v>
       </c>
-      <c r="H55" s="6">
+      <c r="H55" s="15">
         <v>0.4</v>
       </c>
-      <c r="I55" s="6"/>
+      <c r="I55" s="5"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>12</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="15">
         <v>29.25</v>
       </c>
-      <c r="C56" s="6">
+      <c r="C56" s="15">
         <v>29.27</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D56" s="5">
         <v>43.73</v>
       </c>
-      <c r="E56" s="6">
+      <c r="E56" s="5">
         <v>56.69</v>
       </c>
-      <c r="F56" s="6">
+      <c r="F56" s="5">
         <v>52.82</v>
       </c>
-      <c r="G56" s="6">
+      <c r="G56" s="5">
         <v>31.75</v>
       </c>
-      <c r="H56" s="6">
+      <c r="H56" s="15">
         <v>31.72</v>
       </c>
-      <c r="I56" s="6"/>
+      <c r="I56" s="5"/>
     </row>
     <row r="57" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>13</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="9">
         <v>3668</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="9">
         <v>5814</v>
       </c>
       <c r="D57">
@@ -2291,22 +3682,22 @@
       <c r="F57">
         <v>6221</v>
       </c>
-      <c r="G57" s="7">
+      <c r="G57" s="6">
         <v>4265</v>
       </c>
-      <c r="H57" s="8">
+      <c r="H57" s="16">
         <v>4105</v>
       </c>
-      <c r="I57" s="8"/>
+      <c r="I57" s="7"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>14</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="9">
         <v>0</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="9">
         <v>312</v>
       </c>
       <c r="D58">
@@ -2318,13 +3709,13 @@
       <c r="F58">
         <v>252</v>
       </c>
-      <c r="G58" s="8">
+      <c r="G58" s="7">
         <v>0</v>
       </c>
-      <c r="H58" s="8">
+      <c r="H58" s="16">
         <v>0</v>
       </c>
-      <c r="I58" s="8"/>
+      <c r="I58" s="7"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
@@ -2359,7 +3750,10 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C67" t="s">
+      <c r="B67" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D67" t="s">
@@ -2377,7 +3771,7 @@
       <c r="H67" t="s">
         <v>45</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I67" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2385,10 +3779,10 @@
       <c r="A68" t="s">
         <v>10</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="9">
         <v>8.5399999999999991</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="9">
         <v>12.75</v>
       </c>
       <c r="D68">
@@ -2406,7 +3800,7 @@
       <c r="H68">
         <v>8.66</v>
       </c>
-      <c r="I68">
+      <c r="I68" s="9">
         <v>7.85</v>
       </c>
     </row>
@@ -2414,10 +3808,10 @@
       <c r="A69" t="s">
         <v>11</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="9">
         <v>0.08</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="9">
         <v>0.21</v>
       </c>
       <c r="D69">
@@ -2435,7 +3829,7 @@
       <c r="H69">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I69">
+      <c r="I69" s="9">
         <v>0.11</v>
       </c>
     </row>
@@ -2443,10 +3837,10 @@
       <c r="A70" t="s">
         <v>12</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="9">
         <v>29.05</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="9">
         <v>29.08</v>
       </c>
       <c r="D70">
@@ -2464,7 +3858,7 @@
       <c r="H70">
         <v>31.59</v>
       </c>
-      <c r="I70">
+      <c r="I70" s="9">
         <v>31.6</v>
       </c>
     </row>
@@ -2472,10 +3866,10 @@
       <c r="A71" t="s">
         <v>13</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="9">
         <v>3368</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="9">
         <v>3899</v>
       </c>
       <c r="D71">
@@ -2493,7 +3887,7 @@
       <c r="H71">
         <v>4044</v>
       </c>
-      <c r="I71">
+      <c r="I71" s="9">
         <v>3891</v>
       </c>
     </row>
@@ -2501,10 +3895,10 @@
       <c r="A72" t="s">
         <v>14</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="9">
         <v>0</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="9">
         <v>0</v>
       </c>
       <c r="D72">
@@ -2522,9 +3916,14 @@
       <c r="H72">
         <v>0</v>
       </c>
-      <c r="I72">
+      <c r="I72" s="9">
         <v>0</v>
       </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B73" s="9"/>
+      <c r="C73" s="9"/>
+      <c r="I73" s="9"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
@@ -2559,10 +3958,10 @@
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B81" t="s">
+      <c r="B81" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D81" t="s">
@@ -2577,10 +3976,10 @@
       <c r="G81" t="s">
         <v>8</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H81" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I81" t="s">
+      <c r="I81" s="9" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2588,28 +3987,28 @@
       <c r="A82" t="s">
         <v>10</v>
       </c>
-      <c r="B82" s="5">
+      <c r="B82" s="10">
         <v>7.94</v>
       </c>
-      <c r="C82" s="6">
+      <c r="C82" s="15">
         <v>8.5299999999999994</v>
       </c>
-      <c r="D82" s="6">
+      <c r="D82" s="5">
         <v>11.73</v>
       </c>
-      <c r="E82" s="6">
+      <c r="E82" s="5">
         <v>18.91</v>
       </c>
-      <c r="F82" s="6">
+      <c r="F82" s="5">
         <v>11.13</v>
       </c>
-      <c r="G82" s="6">
+      <c r="G82" s="5">
         <v>22.99</v>
       </c>
-      <c r="H82" s="6">
+      <c r="H82" s="15">
         <v>8.16</v>
       </c>
-      <c r="I82" s="6">
+      <c r="I82" s="15">
         <v>7.63</v>
       </c>
     </row>
@@ -2617,28 +4016,28 @@
       <c r="A83" t="s">
         <v>11</v>
       </c>
-      <c r="B83" s="6">
+      <c r="B83" s="15">
         <v>0.4</v>
       </c>
-      <c r="C83" s="6">
+      <c r="C83" s="15">
         <v>0.33</v>
       </c>
-      <c r="D83" s="6">
+      <c r="D83" s="5">
         <v>0.61</v>
       </c>
-      <c r="E83" s="6">
+      <c r="E83" s="5">
         <v>0.8</v>
       </c>
-      <c r="F83" s="6">
+      <c r="F83" s="5">
         <v>0.6</v>
       </c>
-      <c r="G83" s="6">
+      <c r="G83" s="5">
         <v>0.56999999999999995</v>
       </c>
-      <c r="H83" s="6">
+      <c r="H83" s="15">
         <v>0.41</v>
       </c>
-      <c r="I83" s="6">
+      <c r="I83" s="15">
         <v>0.28000000000000003</v>
       </c>
     </row>
@@ -2646,28 +4045,28 @@
       <c r="A84" t="s">
         <v>12</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84" s="15">
         <v>28.74</v>
       </c>
-      <c r="C84" s="6">
+      <c r="C84" s="15">
         <v>28.75</v>
       </c>
-      <c r="D84" s="6">
+      <c r="D84" s="5">
         <v>39.42</v>
       </c>
-      <c r="E84" s="6">
+      <c r="E84" s="5">
         <v>55.15</v>
       </c>
-      <c r="F84" s="6">
+      <c r="F84" s="5">
         <v>51.84</v>
       </c>
-      <c r="G84" s="6">
+      <c r="G84" s="5">
         <v>31.68</v>
       </c>
-      <c r="H84" s="6">
+      <c r="H84" s="15">
         <v>31.71</v>
       </c>
-      <c r="I84" s="6">
+      <c r="I84" s="15">
         <v>31.72</v>
       </c>
     </row>
@@ -2675,10 +4074,10 @@
       <c r="A85" t="s">
         <v>13</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="9">
         <v>3578</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="9">
         <v>3555</v>
       </c>
       <c r="D85">
@@ -2693,10 +4092,10 @@
       <c r="G85">
         <v>4484</v>
       </c>
-      <c r="H85">
+      <c r="H85" s="9">
         <v>4342</v>
       </c>
-      <c r="I85">
+      <c r="I85" s="9">
         <v>4188</v>
       </c>
     </row>
@@ -2704,10 +4103,10 @@
       <c r="A86" t="s">
         <v>14</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="9">
         <v>0</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="9">
         <v>0</v>
       </c>
       <c r="D86">
@@ -2722,12 +4121,16 @@
       <c r="G86">
         <v>10</v>
       </c>
-      <c r="H86">
+      <c r="H86" s="9">
         <v>0</v>
       </c>
-      <c r="I86">
+      <c r="I86" s="9">
         <v>0</v>
       </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B87" s="9"/>
+      <c r="C87" s="9"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
@@ -2789,39 +4192,40 @@
       <c r="J95" t="s">
         <v>55</v>
       </c>
+      <c r="K95" s="9"/>
     </row>
     <row r="96" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>10</v>
       </c>
-      <c r="B96" s="5">
+      <c r="B96" s="10">
         <v>8</v>
       </c>
-      <c r="C96" s="6">
+      <c r="C96" s="15">
         <v>8.7799999999999994</v>
       </c>
-      <c r="D96" s="6">
+      <c r="D96" s="5">
         <v>9.36</v>
       </c>
-      <c r="E96" s="6">
+      <c r="E96" s="5">
         <v>15.3</v>
       </c>
-      <c r="F96" s="6">
+      <c r="F96" s="5">
         <v>8.8000000000000007</v>
       </c>
-      <c r="G96" s="6">
+      <c r="G96" s="5">
         <v>10.84</v>
       </c>
-      <c r="H96" s="6">
+      <c r="H96" s="5">
         <v>11.14</v>
       </c>
-      <c r="I96" s="6">
+      <c r="I96" s="5">
         <v>20.48</v>
       </c>
-      <c r="J96" s="6">
+      <c r="J96" s="5">
         <v>10.18</v>
       </c>
-      <c r="K96" s="6">
+      <c r="K96" s="15">
         <v>6.7130000000000001</v>
       </c>
     </row>
@@ -2829,34 +4233,34 @@
       <c r="A97" t="s">
         <v>11</v>
       </c>
-      <c r="B97" s="6">
+      <c r="B97" s="15">
         <v>0.24</v>
       </c>
-      <c r="C97" s="6">
+      <c r="C97" s="15">
         <v>0.22</v>
       </c>
-      <c r="D97" s="6">
+      <c r="D97" s="5">
         <v>0.22</v>
       </c>
-      <c r="E97" s="6">
+      <c r="E97" s="5">
         <v>0.3</v>
       </c>
-      <c r="F97" s="6">
+      <c r="F97" s="5">
         <v>0.26</v>
       </c>
-      <c r="G97" s="6">
+      <c r="G97" s="5">
         <v>0.24</v>
       </c>
-      <c r="H97" s="6">
+      <c r="H97" s="5">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I97" s="6">
+      <c r="I97" s="5">
         <v>0.42</v>
       </c>
-      <c r="J97" s="6">
+      <c r="J97" s="5">
         <v>0.36</v>
       </c>
-      <c r="K97" s="6">
+      <c r="K97" s="15">
         <v>0.14000000000000001</v>
       </c>
     </row>
@@ -2864,34 +4268,34 @@
       <c r="A98" t="s">
         <v>12</v>
       </c>
-      <c r="B98" s="6">
+      <c r="B98" s="15">
         <v>28.86</v>
       </c>
-      <c r="C98" s="6">
+      <c r="C98" s="15">
         <v>28.86</v>
       </c>
-      <c r="D98" s="6">
+      <c r="D98" s="5">
         <v>45.4</v>
       </c>
-      <c r="E98" s="6">
+      <c r="E98" s="5">
         <v>49.18</v>
       </c>
-      <c r="F98" s="6">
+      <c r="F98" s="5">
         <v>56.86</v>
       </c>
-      <c r="G98" s="6">
+      <c r="G98" s="5">
         <v>56.98</v>
       </c>
-      <c r="H98" s="6">
+      <c r="H98" s="5">
         <v>47.35</v>
       </c>
-      <c r="I98" s="6">
+      <c r="I98" s="5">
         <v>31.5</v>
       </c>
-      <c r="J98" s="6">
+      <c r="J98" s="5">
         <v>31.53</v>
       </c>
-      <c r="K98" s="6">
+      <c r="K98" s="15">
         <v>31.53</v>
       </c>
     </row>
@@ -2899,10 +4303,10 @@
       <c r="A99" t="s">
         <v>13</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="9">
         <v>3513</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="9">
         <v>3535</v>
       </c>
       <c r="D99">
@@ -2926,7 +4330,7 @@
       <c r="J99">
         <v>4478</v>
       </c>
-      <c r="K99">
+      <c r="K99" s="9">
         <v>4088</v>
       </c>
     </row>
@@ -2934,10 +4338,10 @@
       <c r="A100" t="s">
         <v>14</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="9">
         <v>0</v>
       </c>
-      <c r="C100">
+      <c r="C100" s="9">
         <v>255</v>
       </c>
       <c r="D100">
@@ -2961,7 +4365,7 @@
       <c r="J100">
         <v>0</v>
       </c>
-      <c r="K100">
+      <c r="K100" s="9">
         <v>0</v>
       </c>
     </row>
@@ -2998,10 +4402,10 @@
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B109" t="s">
+      <c r="B109" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="9" t="s">
         <v>58</v>
       </c>
       <c r="D109" t="s">
@@ -3019,39 +4423,40 @@
       <c r="H109" t="s">
         <v>63</v>
       </c>
-      <c r="I109" t="s">
+      <c r="I109" s="9" t="s">
         <v>40</v>
       </c>
+      <c r="J109" s="9"/>
     </row>
     <row r="110" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>10</v>
       </c>
-      <c r="B110" s="5">
+      <c r="B110" s="10">
         <v>6.86</v>
       </c>
-      <c r="C110" s="6">
+      <c r="C110" s="15">
         <v>9.69</v>
       </c>
-      <c r="D110" s="6">
+      <c r="D110" s="5">
         <v>12.1</v>
       </c>
-      <c r="E110" s="6">
+      <c r="E110" s="5">
         <v>10.54</v>
       </c>
-      <c r="F110" s="6">
+      <c r="F110" s="5">
         <v>7.82</v>
       </c>
-      <c r="G110" s="6">
+      <c r="G110" s="5">
         <v>8.4499999999999993</v>
       </c>
-      <c r="H110" s="6">
+      <c r="H110" s="5">
         <v>23.25</v>
       </c>
-      <c r="I110" s="6">
+      <c r="I110" s="15">
         <v>8.99</v>
       </c>
-      <c r="J110" s="6">
+      <c r="J110" s="15">
         <v>7.05</v>
       </c>
     </row>
@@ -3059,31 +4464,31 @@
       <c r="A111" t="s">
         <v>11</v>
       </c>
-      <c r="B111" s="6">
+      <c r="B111" s="15">
         <v>0.27</v>
       </c>
-      <c r="C111" s="6">
+      <c r="C111" s="15">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D111" s="6">
+      <c r="D111" s="5">
         <v>0.45</v>
       </c>
-      <c r="E111" s="6">
+      <c r="E111" s="5">
         <v>0.46</v>
       </c>
-      <c r="F111" s="6">
+      <c r="F111" s="5">
         <v>0.48</v>
       </c>
-      <c r="G111" s="6">
+      <c r="G111" s="5">
         <v>0.4</v>
       </c>
-      <c r="H111" s="6">
+      <c r="H111" s="5">
         <v>0.7</v>
       </c>
-      <c r="I111" s="6">
+      <c r="I111" s="15">
         <v>0.52</v>
       </c>
-      <c r="J111" s="6">
+      <c r="J111" s="15">
         <v>0.51</v>
       </c>
     </row>
@@ -3091,31 +4496,31 @@
       <c r="A112" t="s">
         <v>12</v>
       </c>
-      <c r="B112" s="6">
+      <c r="B112" s="15">
         <v>28.94</v>
       </c>
-      <c r="C112" s="6">
+      <c r="C112" s="15">
         <v>36.69</v>
       </c>
-      <c r="D112" s="6">
+      <c r="D112" s="5">
         <v>43.03</v>
       </c>
-      <c r="E112" s="6">
+      <c r="E112" s="5">
         <v>57.49</v>
       </c>
-      <c r="F112" s="6">
+      <c r="F112" s="5">
         <v>58.19</v>
       </c>
-      <c r="G112" s="6">
+      <c r="G112" s="5">
         <v>51.79</v>
       </c>
-      <c r="H112" s="6">
+      <c r="H112" s="5">
         <v>31.59</v>
       </c>
-      <c r="I112" s="6">
+      <c r="I112" s="15">
         <v>31.6</v>
       </c>
-      <c r="J112" s="6">
+      <c r="J112" s="15">
         <v>31.61</v>
       </c>
     </row>
@@ -3123,10 +4528,10 @@
       <c r="A113" t="s">
         <v>13</v>
       </c>
-      <c r="B113">
+      <c r="B113" s="9">
         <v>3586</v>
       </c>
-      <c r="C113">
+      <c r="C113" s="9">
         <v>4978</v>
       </c>
       <c r="D113">
@@ -3144,10 +4549,10 @@
       <c r="H113">
         <v>4325</v>
       </c>
-      <c r="I113">
+      <c r="I113" s="9">
         <v>3800</v>
       </c>
-      <c r="J113">
+      <c r="J113" s="9">
         <v>4063</v>
       </c>
     </row>
@@ -3155,10 +4560,10 @@
       <c r="A114" t="s">
         <v>14</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="9">
         <v>0</v>
       </c>
-      <c r="C114">
+      <c r="C114" s="9">
         <v>308</v>
       </c>
       <c r="D114">
@@ -3176,10 +4581,10 @@
       <c r="H114">
         <v>247</v>
       </c>
-      <c r="I114">
+      <c r="I114" s="9">
         <v>0</v>
       </c>
-      <c r="J114">
+      <c r="J114" s="9">
         <v>0</v>
       </c>
     </row>

</xml_diff>